<commit_message>
decrease cooldown when use hisatsuwaza
</commit_message>
<xml_diff>
--- a/MySurvivorsGame/Assets/StreamingAssets/DevilsData.xlsx
+++ b/MySurvivorsGame/Assets/StreamingAssets/DevilsData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>DevilName</t>
   </si>
@@ -40,6 +40,9 @@
     <t>DropRate</t>
   </si>
   <si>
+    <t>AttackCooldown</t>
+  </si>
+  <si>
     <t>PrefabPath</t>
   </si>
   <si>
@@ -71,6 +74,9 @@
   </si>
   <si>
     <t>寶箱掉落率</t>
+  </si>
+  <si>
+    <t>攻擊冷卻時間</t>
   </si>
   <si>
     <t>下載魔王的prefab</t>
@@ -153,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -166,6 +172,9 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -180,6 +189,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -407,8 +419,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="6" max="6" width="15.25"/>
-    <col customWidth="1" min="10" max="10" width="41.0"/>
-    <col customWidth="1" min="11" max="11" width="16.75"/>
+    <col customWidth="1" min="10" max="10" width="14.63"/>
+    <col customWidth="1" min="11" max="11" width="35.63"/>
     <col customWidth="1" min="12" max="12" width="34.0"/>
   </cols>
   <sheetData>
@@ -440,259 +452,268 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
+      <c r="L1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="F2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="9" t="s">
         <v>20</v>
       </c>
+      <c r="J2" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="K2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
+      <c r="A3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="6">
+      <c r="A4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="7">
         <v>1.2</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>2000.0</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="7">
         <v>3.0</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="7">
         <v>1.0</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="7">
         <v>1.0</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="7">
         <v>5.0</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="7">
         <v>0.0</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="7">
         <v>0.0</v>
       </c>
-      <c r="J4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
+      <c r="J4" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="6">
+      <c r="A5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="7">
         <v>0.7</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="7">
         <v>1000.0</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="7">
         <v>7.0</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="7">
         <v>1.0</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="7">
         <v>1.2</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="7">
         <v>-1.0</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="7">
         <v>0.0</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="7">
         <v>0.0</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="6">
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="7">
         <v>1.0</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7">
         <v>1500.0</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="7">
         <v>5.0</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="7">
         <v>1.2</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="7">
         <v>1.0</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="7">
         <v>0.0</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="7">
         <v>0.0</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="7">
         <v>0.0</v>
       </c>
-      <c r="J6" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="J6" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
     </row>
     <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
     </row>
     <row r="8">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
     </row>
     <row r="9">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
update ChooseItemManager add Weapon to button
</commit_message>
<xml_diff>
--- a/MySurvivorsGame/Assets/StreamingAssets/DevilsData.xlsx
+++ b/MySurvivorsGame/Assets/StreamingAssets/DevilsData.xlsx
@@ -97,7 +97,7 @@
     <t>Assets/Prefabs/Devils/BoneMan.prefab</t>
   </si>
   <si>
-    <t>MagicBallController</t>
+    <t>MagicBall</t>
   </si>
   <si>
     <t>Reaper</t>
@@ -159,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -201,6 +201,9 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -575,13 +578,13 @@
       <c r="I4" s="7">
         <v>0.0</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="7">
         <v>0.9</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="14" t="s">
         <v>28</v>
       </c>
       <c r="M4" s="6"/>
@@ -616,13 +619,13 @@
       <c r="I5" s="7">
         <v>0.0</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="7">
         <v>1.5</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="14" t="s">
         <v>28</v>
       </c>
       <c r="M5" s="6"/>
@@ -657,13 +660,13 @@
       <c r="I6" s="7">
         <v>0.0</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="7">
         <v>1.0</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="14" t="s">
         <v>28</v>
       </c>
       <c r="M6" s="6"/>

</xml_diff>

<commit_message>
update npc HP  = HP * DevilLevel
</commit_message>
<xml_diff>
--- a/MySurvivorsGame/Assets/StreamingAssets/DevilsData.xlsx
+++ b/MySurvivorsGame/Assets/StreamingAssets/DevilsData.xlsx
@@ -611,7 +611,7 @@
         <v>1.2</v>
       </c>
       <c r="G5" s="7">
-        <v>-1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H5" s="7">
         <v>0.0</v>
@@ -652,7 +652,7 @@
         <v>1.0</v>
       </c>
       <c r="G6" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H6" s="7">
         <v>0.0</v>

</xml_diff>